<commit_message>
Trems change Include Infra
</commit_message>
<xml_diff>
--- a/App_Templates/DCRReportTemplate.xlsx
+++ b/App_Templates/DCRReportTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="19155" windowHeight="9015"/>
@@ -16,12 +16,12 @@
   <definedNames>
     <definedName name="Cate">Sheet2!$A$1:$C$24</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>BOILER</t>
   </si>
@@ -165,6 +165,15 @@
   </si>
   <si>
     <t>not requirement</t>
+  </si>
+  <si>
+    <t>GroupID</t>
+  </si>
+  <si>
+    <t>Group Description</t>
+  </si>
+  <si>
+    <t>Discipline</t>
   </si>
 </sst>
 </file>
@@ -588,7 +597,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -916,6 +925,17 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -965,7 +985,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1061,6 +1081,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="23" fillId="38" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="38" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1068,18 +1106,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="38" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="38" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="38" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1154,7 +1180,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-IN"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1181,7 +1207,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1200,11 +1225,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="644484608"/>
-        <c:axId val="619042432"/>
+        <c:axId val="228650496"/>
+        <c:axId val="232880320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="644484608"/>
+        <c:axId val="228650496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1214,7 +1239,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="619042432"/>
+        <c:crossAx val="232880320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1222,7 +1247,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="619042432"/>
+        <c:axId val="232880320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1233,7 +1258,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="644484608"/>
+        <c:crossAx val="228650496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1253,7 +1278,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-IN"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1265,7 +1290,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1684,10 +1708,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="43" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="28"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,43 +1842,58 @@
     <col min="3" max="3" width="14.5703125" style="43" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
       <c r="D2" s="33"/>
       <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
       <c r="D3" s="35"/>
       <c r="E3" s="36"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="37"/>
       <c r="C4" s="24"/>
       <c r="D4" s="31"/>
       <c r="E4" s="32"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>36</v>
       </c>
@@ -1746,131 +1906,52 @@
       <c r="D5" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="26"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="20"/>
       <c r="C6" s="41"/>
       <c r="D6" s="2"/>
       <c r="E6" s="27"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="20"/>
       <c r="C7" s="41"/>
       <c r="D7" s="2"/>
       <c r="E7" s="27"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
       <c r="B8" s="39"/>
       <c r="C8" s="42"/>
       <c r="D8" s="29"/>
       <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="43" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="27"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="27"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B2:C2"/>
   </mergeCells>
@@ -1902,20 +1983,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -2229,20 +2310,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">

</xml_diff>